<commit_message>
JavaScript to move tetrimino down and stop at the end. Created each tetrimino and its rotation
</commit_message>
<xml_diff>
--- a/logic.xlsx
+++ b/logic.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Desktop\TetrisJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4D9635-3771-43E0-97FC-811A4AD546E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A254C613-79E7-4450-84AF-A48E9C048361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{A9F5A8CB-6102-4633-87ED-357E5FB3D3F9}"/>
+    <workbookView xWindow="-14955" yWindow="4245" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{A9F5A8CB-6102-4633-87ED-357E5FB3D3F9}"/>
   </bookViews>
   <sheets>
     <sheet name="grid layout" sheetId="1" r:id="rId1"/>
+    <sheet name="gridPattern" sheetId="2" r:id="rId2"/>
+    <sheet name="rotations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,6 +34,26 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Otetrimino</t>
+  </si>
+  <si>
+    <t>ltetrimino</t>
+  </si>
+  <si>
+    <t>Sktetrimino</t>
+  </si>
+  <si>
+    <t>Stetrimino</t>
+  </si>
+  <si>
+    <t>Ttetrimino</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -43,12 +65,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -143,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -154,6 +182,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,18 +520,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7D2065-6FE0-483F-B6A5-09DDFB33D5FD}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:GZ1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="27" max="208" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="11.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -488,9 +543,9 @@
       <c r="I1" s="3"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="1"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -500,9 +555,9 @@
       <c r="I2" s="1"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -512,7 +567,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -524,7 +579,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -536,7 +591,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="6"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -548,7 +603,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -560,7 +615,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -573,7 +628,7 @@
       <c r="J8" s="6"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -585,7 +640,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -597,7 +652,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -609,7 +664,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -621,7 +676,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -633,7 +688,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -645,7 +700,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -657,7 +712,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -669,7 +724,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -681,7 +736,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -693,7 +748,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -705,7 +760,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -717,10 +772,1198 @@
       <c r="I20" s="8"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:10" ht="11.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FD780E-4C06-4D3C-9AE8-BD484A7172C1}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2" s="12">
+        <v>13</v>
+      </c>
+      <c r="E2" s="12">
+        <v>14</v>
+      </c>
+      <c r="F2" s="12">
+        <v>15</v>
+      </c>
+      <c r="G2" s="12">
+        <v>16</v>
+      </c>
+      <c r="H2" s="12">
+        <v>17</v>
+      </c>
+      <c r="I2" s="12">
+        <v>18</v>
+      </c>
+      <c r="J2" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1">
+        <v>22</v>
+      </c>
+      <c r="D3" s="12">
+        <v>23</v>
+      </c>
+      <c r="E3" s="12">
+        <v>24</v>
+      </c>
+      <c r="F3" s="12">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="C3:J4" si="0">F3+1</f>
+        <v>26</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="J3" s="6">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <f>A3+10</f>
+        <v>30</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A4+1</f>
+        <v>31</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="J4" s="6">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <f t="shared" ref="A5:A19" si="1">A4+10</f>
+        <v>40</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" ref="B5:J20" si="2">A5+1</f>
+        <v>41</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="J5" s="6">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="2"/>
+        <v>77</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="2"/>
+        <v>82</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="2"/>
+        <v>92</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="2"/>
+        <v>93</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="2"/>
+        <v>96</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="2"/>
+        <v>97</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="2"/>
+        <v>98</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="2"/>
+        <v>102</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="E11" s="1">
+        <f t="shared" si="2"/>
+        <v>104</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="2"/>
+        <v>107</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="2"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="2"/>
+        <v>112</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="2"/>
+        <v>113</v>
+      </c>
+      <c r="E12" s="1">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="2"/>
+        <v>117</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="2"/>
+        <v>122</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="2"/>
+        <v>123</v>
+      </c>
+      <c r="E13" s="1">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="2"/>
+        <v>127</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="2"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="2"/>
+        <v>131</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="2"/>
+        <v>142</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="2"/>
+        <v>146</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="2"/>
+        <v>147</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="J15" s="6">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="2"/>
+        <v>152</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="2"/>
+        <v>153</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="2"/>
+        <v>155</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="2"/>
+        <v>158</v>
+      </c>
+      <c r="J16" s="6">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="2"/>
+        <v>161</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="2"/>
+        <v>162</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="2"/>
+        <v>163</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="2"/>
+        <v>164</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="2"/>
+        <v>165</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="2"/>
+        <v>167</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="2"/>
+        <v>168</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="2"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <f t="shared" si="1"/>
+        <v>170</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="2"/>
+        <v>171</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="2"/>
+        <v>172</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="2"/>
+        <v>173</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>174</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="2"/>
+        <v>175</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="2"/>
+        <v>176</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="2"/>
+        <v>177</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="2"/>
+        <v>178</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="2"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="2"/>
+        <v>181</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="2"/>
+        <v>182</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="2"/>
+        <v>183</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="2"/>
+        <v>184</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="2"/>
+        <v>185</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="2"/>
+        <v>186</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="2"/>
+        <v>187</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="2"/>
+        <v>188</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="2"/>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <f>A19+10</f>
+        <v>190</v>
+      </c>
+      <c r="B20" s="8">
+        <f t="shared" si="2"/>
+        <v>191</v>
+      </c>
+      <c r="C20" s="8">
+        <f t="shared" si="2"/>
+        <v>192</v>
+      </c>
+      <c r="D20" s="8">
+        <f t="shared" si="2"/>
+        <v>193</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" si="2"/>
+        <v>194</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="2"/>
+        <v>195</v>
+      </c>
+      <c r="G20" s="8">
+        <f t="shared" si="2"/>
+        <v>196</v>
+      </c>
+      <c r="H20" s="8">
+        <f t="shared" si="2"/>
+        <v>197</v>
+      </c>
+      <c r="I20" s="8">
+        <f t="shared" si="2"/>
+        <v>198</v>
+      </c>
+      <c r="J20" s="9">
+        <f t="shared" si="2"/>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A417C0E-0D53-4161-A89D-DCCFD4F4E149}">
+  <dimension ref="A1:S27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="4"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="4"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="4"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="6"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="6"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="6"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="9"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="9"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="25"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="19"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="19"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="6"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="26"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="21"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="21"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="9"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="27"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="24"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="27"/>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="4"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="26"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="6"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="26"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="28"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="9"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="9"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="9"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="9"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="19"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="26"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="21"/>
+    </row>
+    <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="22"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="24"/>
+    </row>
+    <row r="22" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+    </row>
+    <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+    </row>
+    <row r="24" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="4"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="4"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="4"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="4"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="26"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="26"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="26"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="6"/>
+    </row>
+    <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="9"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="9"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="9"/>
+    </row>
+    <row r="27" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A23:C23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Score increments: need to create gameOver and style appropriately
</commit_message>
<xml_diff>
--- a/logic.xlsx
+++ b/logic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Desktop\TetrisJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A254C613-79E7-4450-84AF-A48E9C048361}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84C6B89-A22E-4D87-96B4-5A68974CF686}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14955" yWindow="4245" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{A9F5A8CB-6102-4633-87ED-357E5FB3D3F9}"/>
   </bookViews>
@@ -1614,7 +1614,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="Z28" sqref="Z28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>